<commit_message>
22.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Price List Update_02.07.2018.xlsx
+++ b/July/Others/Price List Update_02.07.2018.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="94">
   <si>
     <t xml:space="preserve">Model </t>
   </si>
@@ -336,7 +336,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">                    Symphony Price List                           Date:14.07.19   </t>
+    <t>D37</t>
+  </si>
+  <si>
+    <t>BL97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    Symphony Price List                           Date:22.07.19   </t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
       <family val="5"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,6 +510,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,7 +558,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -616,9 +628,6 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="1"/>
@@ -649,6 +658,20 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -959,8 +982,8 @@
   </sheetPr>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -979,60 +1002,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" s="23" customFormat="1" ht="15.75">
       <c r="A5" s="19" t="s">
@@ -1079,17 +1102,17 @@
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="27" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="G6" s="25">
-        <v>1250</v>
+        <v>1200</v>
       </c>
       <c r="H6" s="25">
-        <v>1350</v>
+        <v>1299</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1107,17 +1130,17 @@
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="27" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G7" s="25">
-        <v>1370</v>
+        <v>1250</v>
       </c>
       <c r="H7" s="25">
-        <v>1490</v>
+        <v>1350</v>
       </c>
       <c r="I7" s="26"/>
       <c r="J7" s="26">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1133,17 +1156,17 @@
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="G8" s="25">
-        <v>2780</v>
+        <v>1370</v>
       </c>
       <c r="H8" s="25">
-        <v>2990</v>
+        <v>1490</v>
       </c>
       <c r="I8" s="26"/>
       <c r="J8" s="26">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1161,17 +1184,17 @@
       </c>
       <c r="E9" s="26"/>
       <c r="F9" s="27" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G9" s="25">
-        <v>6540</v>
+        <v>2780</v>
       </c>
       <c r="H9" s="25">
-        <v>6990</v>
+        <v>2990</v>
       </c>
       <c r="I9" s="26"/>
       <c r="J9" s="26">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1189,17 +1212,17 @@
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="27" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="G10" s="25">
-        <v>5290</v>
+        <v>6540</v>
       </c>
       <c r="H10" s="25">
-        <v>5690</v>
+        <v>6990</v>
       </c>
       <c r="I10" s="26"/>
       <c r="J10" s="26">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1217,17 +1240,17 @@
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="27" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="G11" s="25">
-        <v>5470</v>
+        <v>5290</v>
       </c>
       <c r="H11" s="25">
-        <v>5890</v>
+        <v>5690</v>
       </c>
       <c r="I11" s="26"/>
       <c r="J11" s="26">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1245,16 +1268,18 @@
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="27" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="G12" s="25">
-        <v>5750</v>
+        <v>5470</v>
       </c>
       <c r="H12" s="25">
-        <v>6190</v>
+        <v>5890</v>
       </c>
       <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="J12" s="26">
+        <v>70</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="24" t="s">
@@ -1271,18 +1296,16 @@
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="27" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="G13" s="25">
-        <v>5940</v>
+        <v>5750</v>
       </c>
       <c r="H13" s="25">
-        <v>6390</v>
+        <v>6190</v>
       </c>
       <c r="I13" s="26"/>
-      <c r="J13" s="26">
-        <v>90</v>
-      </c>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="24" t="s">
@@ -1299,16 +1322,18 @@
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="27" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="G14" s="25">
-        <v>6530</v>
+        <v>5940</v>
       </c>
       <c r="H14" s="25">
-        <v>6990</v>
+        <v>6390</v>
       </c>
       <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
+      <c r="J14" s="26">
+        <v>90</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="24" t="s">
@@ -1323,20 +1348,16 @@
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
       <c r="F15" s="27" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="G15" s="25">
-        <v>8340</v>
+        <v>6530</v>
       </c>
       <c r="H15" s="25">
-        <v>8990</v>
-      </c>
-      <c r="I15" s="26">
-        <v>500</v>
-      </c>
-      <c r="J15" s="26">
-        <v>100</v>
-      </c>
+        <v>6990</v>
+      </c>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="24" t="s">
@@ -1351,19 +1372,19 @@
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="27" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="G16" s="25">
-        <v>9190</v>
+        <v>8340</v>
       </c>
       <c r="H16" s="25">
-        <v>9990</v>
+        <v>8990</v>
       </c>
       <c r="I16" s="26">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J16" s="26">
-        <v>170</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1381,17 +1402,19 @@
       </c>
       <c r="E17" s="26"/>
       <c r="F17" s="27" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="G17" s="25">
-        <v>5750</v>
+        <v>9190</v>
       </c>
       <c r="H17" s="25">
-        <v>6190</v>
-      </c>
-      <c r="I17" s="26"/>
+        <v>9990</v>
+      </c>
+      <c r="I17" s="26">
+        <v>1000</v>
+      </c>
       <c r="J17" s="26">
-        <v>80</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1409,13 +1432,13 @@
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="27" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="G18" s="25">
-        <v>4640</v>
+        <v>5750</v>
       </c>
       <c r="H18" s="25">
-        <v>4990</v>
+        <v>6190</v>
       </c>
       <c r="I18" s="26"/>
       <c r="J18" s="26">
@@ -1435,17 +1458,19 @@
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
       <c r="F19" s="27" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="G19" s="25">
-        <v>5650</v>
+        <v>4640</v>
       </c>
       <c r="H19" s="25">
-        <v>6150</v>
-      </c>
-      <c r="I19" s="26"/>
+        <v>4990</v>
+      </c>
+      <c r="I19" s="26">
+        <v>200</v>
+      </c>
       <c r="J19" s="26">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1461,44 +1486,44 @@
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
       <c r="F20" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="25">
-        <v>5020</v>
+        <v>5650</v>
       </c>
       <c r="H20" s="25">
-        <v>5390</v>
-      </c>
-      <c r="I20" s="26">
-        <v>200</v>
-      </c>
+        <v>6150</v>
+      </c>
+      <c r="I20" s="26"/>
       <c r="J20" s="26">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="B21" s="25">
-        <v>1000</v>
+        <v>845</v>
       </c>
       <c r="C21" s="25">
-        <v>1090</v>
-      </c>
-      <c r="D21" s="26"/>
+        <v>910</v>
+      </c>
+      <c r="D21" s="26">
+        <v>20</v>
+      </c>
       <c r="E21" s="26"/>
-      <c r="F21" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="25">
-        <v>5280</v>
-      </c>
-      <c r="H21" s="25">
-        <v>5690</v>
-      </c>
-      <c r="I21" s="26">
-        <v>200</v>
+      <c r="F21" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="42">
+        <v>5020</v>
+      </c>
+      <c r="H21" s="42">
+        <v>5390</v>
+      </c>
+      <c r="I21" s="43">
+        <v>400</v>
       </c>
       <c r="J21" s="26">
         <v>100</v>
@@ -1506,505 +1531,515 @@
     </row>
     <row r="22" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="25">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="C22" s="25">
-        <v>1075</v>
+        <v>1090</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
       <c r="F22" s="27" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="G22" s="25">
-        <v>4820</v>
+        <v>5280</v>
       </c>
       <c r="H22" s="25">
-        <v>5190</v>
-      </c>
-      <c r="I22" s="26"/>
+        <v>5690</v>
+      </c>
+      <c r="I22" s="26">
+        <v>200</v>
+      </c>
       <c r="J22" s="26">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="B23" s="25">
-        <v>1000</v>
+        <v>995</v>
       </c>
       <c r="C23" s="25">
-        <v>1090</v>
-      </c>
-      <c r="D23" s="26">
-        <v>10</v>
-      </c>
+        <v>1075</v>
+      </c>
+      <c r="D23" s="26"/>
       <c r="E23" s="26"/>
       <c r="F23" s="27" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="G23" s="25">
-        <v>5100</v>
+        <v>4820</v>
       </c>
       <c r="H23" s="25">
-        <v>5490</v>
-      </c>
-      <c r="I23" s="26">
-        <v>70</v>
-      </c>
-      <c r="J23" s="26"/>
+        <v>5190</v>
+      </c>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26">
+        <v>80</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="27" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="B24" s="25">
-        <v>960</v>
+        <v>880</v>
       </c>
       <c r="C24" s="25">
-        <v>1040</v>
+        <v>950</v>
       </c>
       <c r="D24" s="26">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="28" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="G24" s="25">
-        <v>5560</v>
+        <v>5100</v>
       </c>
       <c r="H24" s="25">
-        <v>5990</v>
+        <v>5490</v>
       </c>
       <c r="I24" s="26">
-        <v>200</v>
-      </c>
-      <c r="J24" s="26">
-        <v>100</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="J24" s="26"/>
     </row>
     <row r="25" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="25">
+        <v>960</v>
+      </c>
+      <c r="C25" s="25">
         <v>1040</v>
       </c>
-      <c r="C25" s="25">
-        <v>1120</v>
-      </c>
       <c r="D25" s="26">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="27" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G25" s="25">
-        <v>6090</v>
+        <v>5560</v>
       </c>
       <c r="H25" s="25">
-        <v>6590</v>
-      </c>
-      <c r="I25" s="26"/>
+        <v>5990</v>
+      </c>
+      <c r="I25" s="26">
+        <v>200</v>
+      </c>
       <c r="J25" s="26">
         <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="24" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="B26" s="25">
-        <v>930</v>
+        <v>1040</v>
       </c>
       <c r="C26" s="25">
-        <v>999</v>
+        <v>1120</v>
       </c>
       <c r="D26" s="26">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="27" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="G26" s="25">
-        <v>5390</v>
+        <v>6090</v>
       </c>
       <c r="H26" s="25">
-        <v>5790</v>
+        <v>6590</v>
       </c>
       <c r="I26" s="26"/>
       <c r="J26" s="26">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="27" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B27" s="25">
-        <v>1290</v>
+        <v>930</v>
       </c>
       <c r="C27" s="25">
-        <v>1390</v>
+        <v>999</v>
       </c>
       <c r="D27" s="26">
         <v>10</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="G27" s="25">
-        <v>3630</v>
+        <v>5390</v>
       </c>
       <c r="H27" s="25">
-        <v>3890</v>
+        <v>5790</v>
       </c>
       <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
+      <c r="J27" s="26">
+        <v>120</v>
+      </c>
     </row>
     <row r="28" spans="1:10" s="10" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="27" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="B28" s="25">
-        <v>1190</v>
+        <v>1290</v>
       </c>
       <c r="C28" s="25">
-        <v>1290</v>
+        <v>1390</v>
       </c>
       <c r="D28" s="26">
         <v>10</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="27" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="G28" s="25">
-        <v>3560</v>
+        <v>3630</v>
       </c>
       <c r="H28" s="25">
-        <v>3840</v>
+        <v>3890</v>
       </c>
       <c r="I28" s="26"/>
-      <c r="J28" s="26">
-        <v>35</v>
-      </c>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="27" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B29" s="25">
-        <v>1270</v>
+        <v>1190</v>
       </c>
       <c r="C29" s="25">
-        <v>1370</v>
+        <v>1290</v>
       </c>
       <c r="D29" s="26">
         <v>10</v>
       </c>
       <c r="E29" s="26"/>
-      <c r="F29" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="25">
-        <v>3340</v>
-      </c>
-      <c r="H29" s="25">
-        <v>3590</v>
-      </c>
-      <c r="I29" s="26"/>
+      <c r="F29" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="42">
+        <v>3560</v>
+      </c>
+      <c r="H29" s="42">
+        <v>3840</v>
+      </c>
+      <c r="I29" s="43">
+        <v>400</v>
+      </c>
       <c r="J29" s="26">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="27" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="B30" s="25">
-        <v>1170</v>
+        <v>1270</v>
       </c>
       <c r="C30" s="25">
-        <v>1270</v>
-      </c>
-      <c r="D30" s="30">
-        <v>10</v>
-      </c>
-      <c r="E30" s="30"/>
-      <c r="F30" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="25">
-        <v>5390</v>
-      </c>
-      <c r="H30" s="25">
-        <v>5790</v>
-      </c>
-      <c r="I30" s="26"/>
+        <v>1370</v>
+      </c>
+      <c r="D30" s="29">
+        <v>10</v>
+      </c>
+      <c r="E30" s="29"/>
+      <c r="F30" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="42">
+        <v>3340</v>
+      </c>
+      <c r="H30" s="42">
+        <v>3590</v>
+      </c>
+      <c r="I30" s="43">
+        <v>320</v>
+      </c>
       <c r="J30" s="26">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="27" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="B31" s="25">
-        <v>1190</v>
+        <v>1170</v>
       </c>
       <c r="C31" s="25">
-        <v>1290</v>
-      </c>
-      <c r="D31" s="31">
-        <v>10</v>
-      </c>
-      <c r="E31" s="31"/>
+        <v>1270</v>
+      </c>
+      <c r="D31" s="30">
+        <v>10</v>
+      </c>
+      <c r="E31" s="30"/>
       <c r="F31" s="27" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="G31" s="25">
-        <v>4500</v>
+        <v>5390</v>
       </c>
       <c r="H31" s="25">
-        <v>4790</v>
+        <v>5790</v>
       </c>
       <c r="I31" s="26"/>
       <c r="J31" s="26">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="27" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="B32" s="25">
-        <v>1225</v>
+        <v>1190</v>
       </c>
       <c r="C32" s="25">
-        <v>1325</v>
-      </c>
-      <c r="D32" s="26"/>
+        <v>1290</v>
+      </c>
+      <c r="D32" s="26">
+        <v>10</v>
+      </c>
       <c r="E32" s="26"/>
       <c r="F32" s="27" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="G32" s="25">
-        <v>4970</v>
+        <v>4500</v>
       </c>
       <c r="H32" s="25">
-        <v>5290</v>
+        <v>4790</v>
       </c>
       <c r="I32" s="26"/>
       <c r="J32" s="26">
-        <v>130</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="27" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B33" s="25">
-        <v>1220</v>
+        <v>1225</v>
       </c>
       <c r="C33" s="25">
-        <v>1320</v>
-      </c>
-      <c r="D33" s="26">
-        <v>20</v>
-      </c>
+        <v>1325</v>
+      </c>
+      <c r="D33" s="26"/>
       <c r="E33" s="26"/>
       <c r="F33" s="27" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="G33" s="25">
-        <v>4015</v>
+        <v>4970</v>
       </c>
       <c r="H33" s="25">
-        <v>4390</v>
+        <v>5290</v>
       </c>
       <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
+      <c r="J33" s="26">
+        <v>130</v>
+      </c>
     </row>
     <row r="34" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="24" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B34" s="25">
-        <v>1080</v>
+        <v>1220</v>
       </c>
       <c r="C34" s="25">
-        <v>1160</v>
+        <v>1320</v>
       </c>
       <c r="D34" s="26">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E34" s="26"/>
-      <c r="F34" s="32" t="s">
-        <v>35</v>
+      <c r="F34" s="31" t="s">
+        <v>62</v>
       </c>
       <c r="G34" s="25">
-        <v>3710</v>
+        <v>4015</v>
       </c>
       <c r="H34" s="25">
-        <v>3990</v>
+        <v>4390</v>
       </c>
       <c r="I34" s="26"/>
-      <c r="J34" s="26">
-        <v>40</v>
-      </c>
+      <c r="J34" s="26"/>
     </row>
     <row r="35" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="25">
-        <v>1100</v>
+        <v>1080</v>
       </c>
       <c r="C35" s="25">
-        <v>1199</v>
+        <v>1160</v>
       </c>
       <c r="D35" s="26">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E35" s="26"/>
-      <c r="F35" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="G35" s="25">
-        <v>3620</v>
-      </c>
-      <c r="H35" s="25">
-        <v>3890</v>
-      </c>
-      <c r="I35" s="30"/>
+      <c r="F35" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="42">
+        <v>3710</v>
+      </c>
+      <c r="H35" s="42">
+        <v>3990</v>
+      </c>
+      <c r="I35" s="44">
+        <v>200</v>
+      </c>
       <c r="J35" s="26">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="27" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="B36" s="25">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="C36" s="25">
-        <v>1290</v>
-      </c>
-      <c r="D36" s="30">
+        <v>1199</v>
+      </c>
+      <c r="D36" s="29">
         <v>20</v>
       </c>
-      <c r="E36" s="30"/>
-      <c r="F36" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="G36" s="25">
-        <v>4620</v>
-      </c>
-      <c r="H36" s="25">
-        <v>4999</v>
-      </c>
-      <c r="I36" s="26"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="42">
+        <v>3620</v>
+      </c>
+      <c r="H36" s="42">
+        <v>3890</v>
+      </c>
+      <c r="I36" s="43">
+        <v>320</v>
+      </c>
       <c r="J36" s="26">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="27" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="B37" s="25">
-        <v>1120</v>
+        <v>1200</v>
       </c>
       <c r="C37" s="25">
-        <v>1220</v>
+        <v>1290</v>
       </c>
       <c r="D37" s="26">
         <v>20</v>
       </c>
       <c r="E37" s="26"/>
       <c r="F37" s="27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G37" s="25">
-        <v>4520</v>
+        <v>4620</v>
       </c>
       <c r="H37" s="25">
-        <v>4899</v>
+        <v>4999</v>
       </c>
       <c r="I37" s="26"/>
       <c r="J37" s="26">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="24" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B38" s="25">
-        <v>1040</v>
+        <v>1120</v>
       </c>
       <c r="C38" s="25">
-        <v>1130</v>
+        <v>1220</v>
       </c>
       <c r="D38" s="26">
         <v>20</v>
       </c>
       <c r="E38" s="26"/>
       <c r="F38" s="27" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G38" s="25">
-        <v>4080</v>
+        <v>4520</v>
       </c>
       <c r="H38" s="25">
-        <v>4390</v>
+        <v>4899</v>
       </c>
       <c r="I38" s="26"/>
       <c r="J38" s="26">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="27" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B39" s="25">
-        <v>1100</v>
+        <v>1040</v>
       </c>
       <c r="C39" s="25">
-        <v>1199</v>
+        <v>1130</v>
       </c>
       <c r="D39" s="26">
         <v>20</v>
       </c>
       <c r="E39" s="26"/>
-      <c r="F39" s="27" t="s">
+      <c r="F39" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" s="42">
+        <v>4080</v>
+      </c>
+      <c r="H39" s="42">
+        <v>4390</v>
+      </c>
+      <c r="I39" s="43">
+        <v>200</v>
+      </c>
+      <c r="J39" s="26">
         <v>70</v>
-      </c>
-      <c r="G39" s="25">
-        <v>4220</v>
-      </c>
-      <c r="H39" s="25">
-        <v>4540</v>
-      </c>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26">
-        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A40" s="27" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B40" s="25">
         <v>1100</v>
@@ -2012,72 +2047,72 @@
       <c r="C40" s="25">
         <v>1199</v>
       </c>
-      <c r="D40" s="26"/>
+      <c r="D40" s="26">
+        <v>20</v>
+      </c>
       <c r="E40" s="26"/>
       <c r="F40" s="27" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="G40" s="25">
-        <v>12240</v>
+        <v>4220</v>
       </c>
       <c r="H40" s="25">
-        <v>12990</v>
+        <v>4540</v>
       </c>
       <c r="I40" s="26"/>
       <c r="J40" s="26">
-        <v>350</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B41" s="25">
-        <v>1050</v>
+        <v>1100</v>
       </c>
       <c r="C41" s="25">
-        <v>1130</v>
-      </c>
-      <c r="D41" s="26">
-        <v>15</v>
-      </c>
+        <v>1199</v>
+      </c>
+      <c r="D41" s="26"/>
       <c r="E41" s="26"/>
       <c r="F41" s="27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G41" s="25">
-        <v>12090</v>
+        <v>12240</v>
       </c>
       <c r="H41" s="25">
         <v>12990</v>
       </c>
       <c r="I41" s="26"/>
       <c r="J41" s="26">
-        <v>200</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="27" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="B42" s="25">
+        <v>1050</v>
+      </c>
+      <c r="C42" s="25">
         <v>1130</v>
       </c>
-      <c r="C42" s="25">
-        <v>1230</v>
-      </c>
       <c r="D42" s="26">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E42" s="26"/>
       <c r="F42" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G42" s="25">
-        <v>10840</v>
+        <v>12090</v>
       </c>
       <c r="H42" s="25">
-        <v>11990</v>
+        <v>12990</v>
       </c>
       <c r="I42" s="26"/>
       <c r="J42" s="26">
@@ -2086,75 +2121,83 @@
     </row>
     <row r="43" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A43" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B43" s="25">
-        <v>1100</v>
+        <v>1130</v>
       </c>
       <c r="C43" s="25">
-        <v>1190</v>
+        <v>1230</v>
       </c>
       <c r="D43" s="26">
         <v>10</v>
       </c>
       <c r="E43" s="26"/>
       <c r="F43" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G43" s="25">
-        <v>12490</v>
+        <v>10840</v>
       </c>
       <c r="H43" s="25">
-        <v>13490</v>
+        <v>11990</v>
       </c>
       <c r="I43" s="26"/>
       <c r="J43" s="26">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="27" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="B44" s="25">
-        <v>1330</v>
+        <v>1100</v>
       </c>
       <c r="C44" s="25">
-        <v>1450</v>
-      </c>
-      <c r="D44" s="26"/>
+        <v>1190</v>
+      </c>
+      <c r="D44" s="26">
+        <v>10</v>
+      </c>
       <c r="E44" s="26"/>
       <c r="F44" s="27" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="G44" s="25">
-        <v>8820</v>
+        <v>12490</v>
       </c>
       <c r="H44" s="25">
-        <v>9490</v>
+        <v>13490</v>
       </c>
       <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="J44" s="26">
+        <v>300</v>
+      </c>
     </row>
     <row r="45" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="27" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="B45" s="25">
-        <v>1200</v>
+        <v>1330</v>
       </c>
       <c r="C45" s="25">
-        <v>1299</v>
-      </c>
-      <c r="D45" s="26">
-        <v>20</v>
-      </c>
+        <v>1450</v>
+      </c>
+      <c r="D45" s="26"/>
       <c r="E45" s="26"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="F45" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="40">
+        <v>8820</v>
+      </c>
+      <c r="H45" s="40">
+        <v>9490</v>
+      </c>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10">
       <c r="F46" s="6"/>
@@ -2210,60 +2253,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="46.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18.75">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="19.5">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="37.5">
       <c r="A5" s="2" t="s">

</xml_diff>